<commit_message>
Auto commit at 2025-10-02 15:28:58.93
</commit_message>
<xml_diff>
--- a/data/yhxw.xlsx
+++ b/data/yhxw.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -478,15 +478,17 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="K74" sqref="K74"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="13.125" style="3" customWidth="1"/>
     <col min="2" max="2" width="18.125" customWidth="1"/>
-    <col min="3" max="26" width="10.25" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.25" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="26" width="10.25" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15" x14ac:dyDescent="0.25">
@@ -4486,7 +4488,7 @@
         <v>0</v>
       </c>
       <c r="Z50" s="5">
-        <v>0</v>
+        <v>17.177</v>
       </c>
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.15">
@@ -4566,7 +4568,7 @@
         <v>0</v>
       </c>
       <c r="Z51" s="5">
-        <v>58.469000000000001</v>
+        <v>68.25</v>
       </c>
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.15">
@@ -4646,7 +4648,7 @@
         <v>108.33</v>
       </c>
       <c r="Z52" s="5">
-        <v>0</v>
+        <v>18.091999999999999</v>
       </c>
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.15">
@@ -4966,7 +4968,7 @@
         <v>170.19</v>
       </c>
       <c r="Z56" s="5">
-        <v>85.036000000000001</v>
+        <v>93.575999999999993</v>
       </c>
     </row>
     <row r="57" spans="1:26" x14ac:dyDescent="0.15">
@@ -5046,7 +5048,7 @@
         <v>142.423</v>
       </c>
       <c r="Z57" s="5">
-        <v>0</v>
+        <v>5.7889999999999997</v>
       </c>
     </row>
     <row r="58" spans="1:26" x14ac:dyDescent="0.15">
@@ -5126,7 +5128,7 @@
         <v>19.100000000000001</v>
       </c>
       <c r="Z58" s="5">
-        <v>124.51000000000002</v>
+        <v>142.13800000000001</v>
       </c>
     </row>
     <row r="59" spans="1:26" x14ac:dyDescent="0.15">
@@ -5206,7 +5208,7 @@
         <v>43.75</v>
       </c>
       <c r="Z59" s="5">
-        <v>5.484</v>
+        <v>13.225999999999999</v>
       </c>
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Auto commit at 2025-10-02 15:50:53.00
</commit_message>
<xml_diff>
--- a/data/yhxw.xlsx
+++ b/data/yhxw.xlsx
@@ -478,8 +478,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="J72" sqref="J72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5368,7 +5368,7 @@
         <v>130.91400000000002</v>
       </c>
       <c r="Z61" s="5">
-        <v>55.676000000000002</v>
+        <v>87.227000000000004</v>
       </c>
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.15">
@@ -5528,7 +5528,7 @@
         <v>0</v>
       </c>
       <c r="Z63" s="5">
-        <v>0</v>
+        <v>29.593</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto commit at 2026-02-25  9:32:24.79
</commit_message>
<xml_diff>
--- a/data/yhxw.xlsx
+++ b/data/yhxw.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="31">
   <si>
     <t>日期</t>
   </si>
@@ -106,6 +106,9 @@
   <si>
     <t>高岭站充电量(kw)</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2026-2-29</t>
   </si>
 </sst>
 </file>
@@ -478,8 +481,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z293"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A250" workbookViewId="0">
-      <selection activeCell="F294" sqref="F294"/>
+    <sheetView tabSelected="1" topLeftCell="A236" workbookViewId="0">
+      <selection activeCell="B251" sqref="B251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -20093,7 +20096,7 @@
     </row>
     <row r="246" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A246" s="3">
-        <v>46023</v>
+        <v>46054</v>
       </c>
       <c r="B246" t="s">
         <v>26</v>
@@ -20173,7 +20176,7 @@
     </row>
     <row r="247" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A247" s="3">
-        <v>46023</v>
+        <v>46054</v>
       </c>
       <c r="B247" t="s">
         <v>27</v>
@@ -20253,7 +20256,7 @@
     </row>
     <row r="248" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A248" s="3">
-        <v>46024</v>
+        <v>46055</v>
       </c>
       <c r="B248" t="s">
         <v>26</v>
@@ -20333,7 +20336,7 @@
     </row>
     <row r="249" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A249" s="3">
-        <v>46024</v>
+        <v>46055</v>
       </c>
       <c r="B249" t="s">
         <v>27</v>
@@ -20413,7 +20416,7 @@
     </row>
     <row r="250" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A250" s="3">
-        <v>46025</v>
+        <v>46056</v>
       </c>
       <c r="B250" t="s">
         <v>26</v>
@@ -20493,7 +20496,7 @@
     </row>
     <row r="251" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A251" s="3">
-        <v>46025</v>
+        <v>46056</v>
       </c>
       <c r="B251" t="s">
         <v>27</v>
@@ -20573,7 +20576,7 @@
     </row>
     <row r="252" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A252" s="3">
-        <v>46026</v>
+        <v>46057</v>
       </c>
       <c r="B252" t="s">
         <v>26</v>
@@ -20653,7 +20656,7 @@
     </row>
     <row r="253" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A253" s="3">
-        <v>46026</v>
+        <v>46057</v>
       </c>
       <c r="B253" t="s">
         <v>27</v>
@@ -20733,7 +20736,7 @@
     </row>
     <row r="254" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A254" s="3">
-        <v>46027</v>
+        <v>46058</v>
       </c>
       <c r="B254" t="s">
         <v>26</v>
@@ -20813,7 +20816,7 @@
     </row>
     <row r="255" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A255" s="3">
-        <v>46027</v>
+        <v>46058</v>
       </c>
       <c r="B255" t="s">
         <v>27</v>
@@ -20893,7 +20896,7 @@
     </row>
     <row r="256" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A256" s="3">
-        <v>46028</v>
+        <v>46059</v>
       </c>
       <c r="B256" t="s">
         <v>26</v>
@@ -20973,7 +20976,7 @@
     </row>
     <row r="257" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A257" s="3">
-        <v>46028</v>
+        <v>46059</v>
       </c>
       <c r="B257" t="s">
         <v>27</v>
@@ -21053,7 +21056,7 @@
     </row>
     <row r="258" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A258" s="3">
-        <v>46029</v>
+        <v>46060</v>
       </c>
       <c r="B258" t="s">
         <v>26</v>
@@ -21133,7 +21136,7 @@
     </row>
     <row r="259" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A259" s="3">
-        <v>46029</v>
+        <v>46060</v>
       </c>
       <c r="B259" t="s">
         <v>27</v>
@@ -21213,7 +21216,7 @@
     </row>
     <row r="260" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A260" s="3">
-        <v>46030</v>
+        <v>46061</v>
       </c>
       <c r="B260" t="s">
         <v>26</v>
@@ -21293,7 +21296,7 @@
     </row>
     <row r="261" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A261" s="3">
-        <v>46030</v>
+        <v>46061</v>
       </c>
       <c r="B261" t="s">
         <v>27</v>
@@ -21373,7 +21376,7 @@
     </row>
     <row r="262" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A262" s="3">
-        <v>46031</v>
+        <v>46062</v>
       </c>
       <c r="B262" t="s">
         <v>26</v>
@@ -21453,7 +21456,7 @@
     </row>
     <row r="263" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A263" s="3">
-        <v>46031</v>
+        <v>46062</v>
       </c>
       <c r="B263" t="s">
         <v>27</v>
@@ -21533,7 +21536,7 @@
     </row>
     <row r="264" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A264" s="3">
-        <v>46032</v>
+        <v>46073</v>
       </c>
       <c r="B264" t="s">
         <v>26</v>
@@ -21613,7 +21616,7 @@
     </row>
     <row r="265" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A265" s="3">
-        <v>46032</v>
+        <v>46073</v>
       </c>
       <c r="B265" t="s">
         <v>27</v>
@@ -21693,7 +21696,7 @@
     </row>
     <row r="266" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A266" s="3">
-        <v>46033</v>
+        <v>46075</v>
       </c>
       <c r="B266" t="s">
         <v>26</v>
@@ -21773,7 +21776,7 @@
     </row>
     <row r="267" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A267" s="3">
-        <v>46033</v>
+        <v>46075</v>
       </c>
       <c r="B267" t="s">
         <v>27</v>
@@ -21853,7 +21856,7 @@
     </row>
     <row r="268" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A268" s="3">
-        <v>46034</v>
+        <v>46075</v>
       </c>
       <c r="B268" t="s">
         <v>26</v>
@@ -21933,7 +21936,7 @@
     </row>
     <row r="269" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A269" s="3">
-        <v>46034</v>
+        <v>46075</v>
       </c>
       <c r="B269" t="s">
         <v>27</v>
@@ -22013,7 +22016,7 @@
     </row>
     <row r="270" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A270" s="3">
-        <v>46035</v>
+        <v>46076</v>
       </c>
       <c r="B270" t="s">
         <v>26</v>
@@ -22093,7 +22096,7 @@
     </row>
     <row r="271" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A271" s="3">
-        <v>46035</v>
+        <v>46076</v>
       </c>
       <c r="B271" t="s">
         <v>27</v>
@@ -22173,7 +22176,7 @@
     </row>
     <row r="272" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A272" s="3">
-        <v>46036</v>
+        <v>46077</v>
       </c>
       <c r="B272" t="s">
         <v>26</v>
@@ -22253,7 +22256,7 @@
     </row>
     <row r="273" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A273" s="3">
-        <v>46036</v>
+        <v>46077</v>
       </c>
       <c r="B273" t="s">
         <v>27</v>
@@ -22333,7 +22336,7 @@
     </row>
     <row r="274" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A274" s="3">
-        <v>46037</v>
+        <v>46078</v>
       </c>
       <c r="B274" t="s">
         <v>26</v>
@@ -22413,7 +22416,7 @@
     </row>
     <row r="275" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A275" s="3">
-        <v>46037</v>
+        <v>46078</v>
       </c>
       <c r="B275" t="s">
         <v>27</v>
@@ -22493,7 +22496,7 @@
     </row>
     <row r="276" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A276" s="3">
-        <v>46038</v>
+        <v>46079</v>
       </c>
       <c r="B276" t="s">
         <v>26</v>
@@ -22573,7 +22576,7 @@
     </row>
     <row r="277" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A277" s="3">
-        <v>46038</v>
+        <v>46079</v>
       </c>
       <c r="B277" t="s">
         <v>27</v>
@@ -22653,7 +22656,7 @@
     </row>
     <row r="278" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A278" s="3">
-        <v>46039</v>
+        <v>46080</v>
       </c>
       <c r="B278" t="s">
         <v>26</v>
@@ -22733,7 +22736,7 @@
     </row>
     <row r="279" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A279" s="3">
-        <v>46039</v>
+        <v>46080</v>
       </c>
       <c r="B279" t="s">
         <v>27</v>
@@ -22813,7 +22816,7 @@
     </row>
     <row r="280" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A280" s="3">
-        <v>46040</v>
+        <v>46081</v>
       </c>
       <c r="B280" t="s">
         <v>26</v>
@@ -22893,7 +22896,7 @@
     </row>
     <row r="281" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A281" s="3">
-        <v>46040</v>
+        <v>46081</v>
       </c>
       <c r="B281" t="s">
         <v>27</v>
@@ -22972,8 +22975,8 @@
       </c>
     </row>
     <row r="282" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A282" s="3">
-        <v>46041</v>
+      <c r="A282" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B282" t="s">
         <v>26</v>
@@ -23052,8 +23055,8 @@
       </c>
     </row>
     <row r="283" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A283" s="3">
-        <v>46041</v>
+      <c r="A283" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B283" t="s">
         <v>27</v>
@@ -23133,7 +23136,7 @@
     </row>
     <row r="284" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A284" s="3">
-        <v>46042</v>
+        <v>46073</v>
       </c>
       <c r="B284" t="s">
         <v>26</v>
@@ -23213,7 +23216,7 @@
     </row>
     <row r="285" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A285" s="3">
-        <v>46042</v>
+        <v>46073</v>
       </c>
       <c r="B285" t="s">
         <v>27</v>
@@ -23293,7 +23296,7 @@
     </row>
     <row r="286" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A286" s="3">
-        <v>46043</v>
+        <v>46075</v>
       </c>
       <c r="B286" t="s">
         <v>26</v>
@@ -23373,7 +23376,7 @@
     </row>
     <row r="287" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A287" s="3">
-        <v>46043</v>
+        <v>46075</v>
       </c>
       <c r="B287" t="s">
         <v>27</v>
@@ -23453,7 +23456,7 @@
     </row>
     <row r="288" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A288" s="3">
-        <v>46044</v>
+        <v>46075</v>
       </c>
       <c r="B288" t="s">
         <v>26</v>
@@ -23533,7 +23536,7 @@
     </row>
     <row r="289" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A289" s="3">
-        <v>46044</v>
+        <v>46075</v>
       </c>
       <c r="B289" t="s">
         <v>27</v>
@@ -23613,7 +23616,7 @@
     </row>
     <row r="290" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A290" s="3">
-        <v>46045</v>
+        <v>46076</v>
       </c>
       <c r="B290" t="s">
         <v>26</v>
@@ -23693,7 +23696,7 @@
     </row>
     <row r="291" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A291" s="3">
-        <v>46045</v>
+        <v>46076</v>
       </c>
       <c r="B291" t="s">
         <v>27</v>
@@ -23773,7 +23776,7 @@
     </row>
     <row r="292" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A292" s="3">
-        <v>46046</v>
+        <v>46077</v>
       </c>
       <c r="B292" t="s">
         <v>26</v>
@@ -23853,7 +23856,7 @@
     </row>
     <row r="293" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A293" s="3">
-        <v>46046</v>
+        <v>46077</v>
       </c>
       <c r="B293" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Auto commit at 2026-02-25  9:58:10.29
</commit_message>
<xml_diff>
--- a/data/yhxw.xlsx
+++ b/data/yhxw.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="30">
   <si>
     <t>日期</t>
   </si>
@@ -106,9 +106,6 @@
   <si>
     <t>高岭站充电量(kw)</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2026-2-29</t>
   </si>
 </sst>
 </file>
@@ -481,8 +478,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z293"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A236" workbookViewId="0">
-      <selection activeCell="B251" sqref="B251"/>
+    <sheetView tabSelected="1" topLeftCell="A257" workbookViewId="0">
+      <selection activeCell="B288" sqref="B288"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -21536,7 +21533,7 @@
     </row>
     <row r="264" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A264" s="3">
-        <v>46073</v>
+        <v>46063</v>
       </c>
       <c r="B264" t="s">
         <v>26</v>
@@ -21616,7 +21613,7 @@
     </row>
     <row r="265" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A265" s="3">
-        <v>46073</v>
+        <v>46063</v>
       </c>
       <c r="B265" t="s">
         <v>27</v>
@@ -21696,7 +21693,7 @@
     </row>
     <row r="266" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A266" s="3">
-        <v>46075</v>
+        <v>46064</v>
       </c>
       <c r="B266" t="s">
         <v>26</v>
@@ -21776,7 +21773,7 @@
     </row>
     <row r="267" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A267" s="3">
-        <v>46075</v>
+        <v>46064</v>
       </c>
       <c r="B267" t="s">
         <v>27</v>
@@ -21856,7 +21853,7 @@
     </row>
     <row r="268" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A268" s="3">
-        <v>46075</v>
+        <v>46065</v>
       </c>
       <c r="B268" t="s">
         <v>26</v>
@@ -21936,7 +21933,7 @@
     </row>
     <row r="269" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A269" s="3">
-        <v>46075</v>
+        <v>46065</v>
       </c>
       <c r="B269" t="s">
         <v>27</v>
@@ -22016,7 +22013,7 @@
     </row>
     <row r="270" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A270" s="3">
-        <v>46076</v>
+        <v>46066</v>
       </c>
       <c r="B270" t="s">
         <v>26</v>
@@ -22096,7 +22093,7 @@
     </row>
     <row r="271" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A271" s="3">
-        <v>46076</v>
+        <v>46066</v>
       </c>
       <c r="B271" t="s">
         <v>27</v>
@@ -22176,7 +22173,7 @@
     </row>
     <row r="272" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A272" s="3">
-        <v>46077</v>
+        <v>46067</v>
       </c>
       <c r="B272" t="s">
         <v>26</v>
@@ -22256,7 +22253,7 @@
     </row>
     <row r="273" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A273" s="3">
-        <v>46077</v>
+        <v>46067</v>
       </c>
       <c r="B273" t="s">
         <v>27</v>
@@ -22336,7 +22333,7 @@
     </row>
     <row r="274" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A274" s="3">
-        <v>46078</v>
+        <v>46068</v>
       </c>
       <c r="B274" t="s">
         <v>26</v>
@@ -22416,7 +22413,7 @@
     </row>
     <row r="275" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A275" s="3">
-        <v>46078</v>
+        <v>46068</v>
       </c>
       <c r="B275" t="s">
         <v>27</v>
@@ -22496,7 +22493,7 @@
     </row>
     <row r="276" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A276" s="3">
-        <v>46079</v>
+        <v>46069</v>
       </c>
       <c r="B276" t="s">
         <v>26</v>
@@ -22576,7 +22573,7 @@
     </row>
     <row r="277" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A277" s="3">
-        <v>46079</v>
+        <v>46069</v>
       </c>
       <c r="B277" t="s">
         <v>27</v>
@@ -22656,7 +22653,7 @@
     </row>
     <row r="278" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A278" s="3">
-        <v>46080</v>
+        <v>46070</v>
       </c>
       <c r="B278" t="s">
         <v>26</v>
@@ -22736,7 +22733,7 @@
     </row>
     <row r="279" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A279" s="3">
-        <v>46080</v>
+        <v>46070</v>
       </c>
       <c r="B279" t="s">
         <v>27</v>
@@ -22816,7 +22813,7 @@
     </row>
     <row r="280" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A280" s="3">
-        <v>46081</v>
+        <v>46071</v>
       </c>
       <c r="B280" t="s">
         <v>26</v>
@@ -22896,7 +22893,7 @@
     </row>
     <row r="281" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A281" s="3">
-        <v>46081</v>
+        <v>46071</v>
       </c>
       <c r="B281" t="s">
         <v>27</v>
@@ -22975,8 +22972,8 @@
       </c>
     </row>
     <row r="282" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A282" s="3" t="s">
-        <v>30</v>
+      <c r="A282" s="3">
+        <v>46072</v>
       </c>
       <c r="B282" t="s">
         <v>26</v>
@@ -23055,8 +23052,8 @@
       </c>
     </row>
     <row r="283" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="A283" s="3" t="s">
-        <v>30</v>
+      <c r="A283" s="3">
+        <v>46072</v>
       </c>
       <c r="B283" t="s">
         <v>27</v>
@@ -23296,7 +23293,7 @@
     </row>
     <row r="286" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A286" s="3">
-        <v>46075</v>
+        <v>46074</v>
       </c>
       <c r="B286" t="s">
         <v>26</v>
@@ -23376,7 +23373,7 @@
     </row>
     <row r="287" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A287" s="3">
-        <v>46075</v>
+        <v>46074</v>
       </c>
       <c r="B287" t="s">
         <v>27</v>

</xml_diff>